<commit_message>
new hawaii file, changed q-fit plot legend
</commit_message>
<xml_diff>
--- a/rawdata/TableHawaii.xlsx
+++ b/rawdata/TableHawaii.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\geologia\punticaldi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7DE75A-237C-4D8E-BCE5-D1568F001400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E95575-6942-48F2-8E84-5D5A04DE37AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD9ED927-770F-4074-ACE8-AFC6CB6EA1C9}"/>
   </bookViews>
@@ -481,7 +481,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G63" sqref="G63"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
         <v>30787</v>
       </c>
       <c r="L3">
-        <v>4.0518096005949744E-2</v>
+        <v>4.0516826173393999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
@@ -602,19 +602,19 @@
         <v>2</v>
       </c>
       <c r="H4">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4">
         <v>61</v>
       </c>
-      <c r="J4" s="6">
-        <v>31589</v>
+      <c r="J4" s="9">
+        <v>30787</v>
       </c>
       <c r="K4" s="5">
         <v>43317</v>
       </c>
       <c r="L4">
-        <v>0.21353546371896856</v>
+        <v>0.19986783</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>